<commit_message>
8-setting data so that it runs against a single line
</commit_message>
<xml_diff>
--- a/Resources/8-data.xlsx
+++ b/Resources/8-data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="960" yWindow="660" windowWidth="27315" windowHeight="11760"/>
+    <workbookView xWindow="960" yWindow="660" windowWidth="24240" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -373,10 +373,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -405,35 +405,35 @@
         <v>904492748</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>3013684370</v>
-      </c>
-      <c r="B3">
-        <v>904492469</v>
-      </c>
-    </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>3013688560</v>
+        <v>3013684370</v>
       </c>
       <c r="B4">
-        <v>904493578</v>
+        <v>904492469</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>3013686777</v>
+        <v>3013688560</v>
       </c>
       <c r="B5">
-        <v>904493242</v>
+        <v>904493578</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
+        <v>3013686777</v>
+      </c>
+      <c r="B6">
+        <v>904493242</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
         <v>3013686776</v>
       </c>
-      <c r="B6">
+      <c r="B7">
         <v>904493314</v>
       </c>
     </row>

</xml_diff>

<commit_message>
8- Added data and code to read latest data From excel
</commit_message>
<xml_diff>
--- a/Resources/8-data.xlsx
+++ b/Resources/8-data.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="960" yWindow="660" windowWidth="20580" windowHeight="11640" activeTab="1"/>
+    <workbookView xWindow="960" yWindow="660" windowWidth="20580" windowHeight="11640"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Old Invoices" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="910" uniqueCount="271">
   <si>
     <t>ORDER</t>
   </si>
@@ -529,6 +530,306 @@
   </si>
   <si>
     <t xml:space="preserve">Players 14 Stand Bag Custom                                 </t>
+  </si>
+  <si>
+    <t>904845552</t>
+  </si>
+  <si>
+    <t>20171025</t>
+  </si>
+  <si>
+    <t>3013953706</t>
+  </si>
+  <si>
+    <t>14258881</t>
+  </si>
+  <si>
+    <t>US00026239</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pom Pom Winter Hat Asst.      </t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>15.00</t>
+  </si>
+  <si>
+    <t>0.00</t>
+  </si>
+  <si>
+    <t>90.00</t>
+  </si>
+  <si>
+    <t>6.39</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 90.00</t>
+  </si>
+  <si>
+    <t>904845630</t>
+  </si>
+  <si>
+    <t>3013996080</t>
+  </si>
+  <si>
+    <t>14446757</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WASHINGTON DUKE     </t>
+  </si>
+  <si>
+    <t>USEE000001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TA5TVWRLR      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pro Wheeled Roller Bag Black  </t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>180.00</t>
+  </si>
+  <si>
+    <t>100.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.00</t>
+  </si>
+  <si>
+    <t>904845629</t>
+  </si>
+  <si>
+    <t>3013996079</t>
+  </si>
+  <si>
+    <t>14446756</t>
+  </si>
+  <si>
+    <t>USEM000044</t>
+  </si>
+  <si>
+    <t>904845557</t>
+  </si>
+  <si>
+    <t>3013965607</t>
+  </si>
+  <si>
+    <t>14320931</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POM/POMS            </t>
+  </si>
+  <si>
+    <t>US00033077</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>8.78</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 180.00</t>
+  </si>
+  <si>
+    <t>904845587</t>
+  </si>
+  <si>
+    <t>3013996644</t>
+  </si>
+  <si>
+    <t>14447662</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CUSTOM              </t>
+  </si>
+  <si>
+    <t xml:space="preserve">TA5ACMFTWLC    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Waffle Microfiber Towel CST   </t>
+  </si>
+  <si>
+    <t>17.00</t>
+  </si>
+  <si>
+    <t>9.07</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 17.00</t>
+  </si>
+  <si>
+    <t>904845652</t>
+  </si>
+  <si>
+    <t>3013996239</t>
+  </si>
+  <si>
+    <t>14446940</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CART MITTS          </t>
+  </si>
+  <si>
+    <t>US00059139</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TA7WEACM-0     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Titleist Cart Mitts           </t>
+  </si>
+  <si>
+    <t>22.50</t>
+  </si>
+  <si>
+    <t>135.00</t>
+  </si>
+  <si>
+    <t>9.98</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 135.00</t>
+  </si>
+  <si>
+    <t>904845551</t>
+  </si>
+  <si>
+    <t>3013953151</t>
+  </si>
+  <si>
+    <t>14257783</t>
+  </si>
+  <si>
+    <t>US00031646</t>
+  </si>
+  <si>
+    <t>9.11</t>
+  </si>
+  <si>
+    <t>904845583</t>
+  </si>
+  <si>
+    <t>3013995773</t>
+  </si>
+  <si>
+    <t>14446306</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S                   </t>
+  </si>
+  <si>
+    <t>US00060065</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TH7VTP-P12     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tour Perf Visor Legacy Asst   </t>
+  </si>
+  <si>
+    <t>12.00</t>
+  </si>
+  <si>
+    <t>8.00</t>
+  </si>
+  <si>
+    <t>96.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 96.00</t>
+  </si>
+  <si>
+    <t>904845651</t>
+  </si>
+  <si>
+    <t>3013996237</t>
+  </si>
+  <si>
+    <t>14446939</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WINTER CAPS         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lifestyle Beanie Legacy Asst  </t>
+  </si>
+  <si>
+    <t>12.50</t>
+  </si>
+  <si>
+    <t>75.00</t>
+  </si>
+  <si>
+    <t>8.39</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 75.00</t>
+  </si>
+  <si>
+    <t>904845581</t>
+  </si>
+  <si>
+    <t>3013995485</t>
+  </si>
+  <si>
+    <t>14445845</t>
+  </si>
+  <si>
+    <t xml:space="preserve">THOMAS              </t>
+  </si>
+  <si>
+    <t>US00002681</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TH7ASC-P06     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tour Snapback Asst.           </t>
+  </si>
+  <si>
+    <t>904845578</t>
+  </si>
+  <si>
+    <t>3013995270</t>
+  </si>
+  <si>
+    <t>14445144</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WLA001716-27        </t>
+  </si>
+  <si>
+    <t>US00057861</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TA1ACFVP-0     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fleece Valuables Pouch        </t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>6.00</t>
+  </si>
+  <si>
+    <t>2.00</t>
+  </si>
+  <si>
+    <t>5.88</t>
+  </si>
+  <si>
+    <t>23.52</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 23.52</t>
   </si>
 </sst>
 </file>
@@ -645,7 +946,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -668,6 +969,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -969,68 +1272,852 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:V12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" customWidth="1"/>
+    <col min="1" max="1" width="12.28515625" style="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" style="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" style="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.140625" style="21" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" style="21" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.140625" style="21" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" style="21" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" style="21" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.28515625" style="21" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.28515625" style="21" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.85546875" style="21" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.7109375" style="21" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="6" style="21" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.5703125" style="21" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11" style="21" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.85546875" style="21" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.140625" style="21" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18.5703125" style="21" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17" style="21" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="30.42578125" style="21" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.5703125" style="21" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="9.140625" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>3013686313</v>
-      </c>
-      <c r="B2">
-        <v>904492748</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3013684370</v>
-      </c>
-      <c r="B4">
-        <v>904492469</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>3013688560</v>
-      </c>
-      <c r="B5">
-        <v>904493578</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>3013686777</v>
-      </c>
-      <c r="B6">
-        <v>904493242</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>3013686776</v>
-      </c>
-      <c r="B7">
-        <v>904493314</v>
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A1" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="M1" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="N1" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="O1" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="P1" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q1" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="R1" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="S1" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="T1" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="U1" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="V1" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A2" s="21" t="s">
+        <v>171</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>172</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>173</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>174</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="G2" s="21" t="s">
+        <v>175</v>
+      </c>
+      <c r="H2" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" s="21" t="s">
+        <v>176</v>
+      </c>
+      <c r="J2" s="21" t="s">
+        <v>177</v>
+      </c>
+      <c r="K2" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="L2" s="21" t="s">
+        <v>178</v>
+      </c>
+      <c r="M2" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="N2" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="O2" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="P2" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="Q2" s="21" t="s">
+        <v>178</v>
+      </c>
+      <c r="R2" s="21" t="s">
+        <v>180</v>
+      </c>
+      <c r="S2" s="21" t="s">
+        <v>177</v>
+      </c>
+      <c r="T2" s="21" t="s">
+        <v>180</v>
+      </c>
+      <c r="U2" s="21" t="s">
+        <v>181</v>
+      </c>
+      <c r="V2" s="21" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A3" s="21" t="s">
+        <v>183</v>
+      </c>
+      <c r="B3" s="21" t="s">
+        <v>172</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>184</v>
+      </c>
+      <c r="D3" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="21" t="s">
+        <v>185</v>
+      </c>
+      <c r="F3" s="21" t="s">
+        <v>186</v>
+      </c>
+      <c r="G3" s="21" t="s">
+        <v>187</v>
+      </c>
+      <c r="H3" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="I3" s="21" t="s">
+        <v>189</v>
+      </c>
+      <c r="J3" s="21" t="s">
+        <v>190</v>
+      </c>
+      <c r="K3" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="L3" s="21" t="s">
+        <v>191</v>
+      </c>
+      <c r="M3" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="N3" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="O3" s="21" t="s">
+        <v>192</v>
+      </c>
+      <c r="P3" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="Q3" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="R3" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="S3" s="21" t="s">
+        <v>190</v>
+      </c>
+      <c r="T3" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="U3" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="V3" s="21" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A4" s="21" t="s">
+        <v>194</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>172</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>195</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="21" t="s">
+        <v>196</v>
+      </c>
+      <c r="F4" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="G4" s="21" t="s">
+        <v>197</v>
+      </c>
+      <c r="H4" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="I4" s="21" t="s">
+        <v>189</v>
+      </c>
+      <c r="J4" s="21" t="s">
+        <v>190</v>
+      </c>
+      <c r="K4" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="L4" s="21" t="s">
+        <v>191</v>
+      </c>
+      <c r="M4" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="N4" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="O4" s="21" t="s">
+        <v>192</v>
+      </c>
+      <c r="P4" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="Q4" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="R4" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="S4" s="21" t="s">
+        <v>190</v>
+      </c>
+      <c r="T4" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="U4" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="V4" s="21" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A5" s="21" t="s">
+        <v>198</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>172</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>199</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="21" t="s">
+        <v>200</v>
+      </c>
+      <c r="F5" s="21" t="s">
+        <v>201</v>
+      </c>
+      <c r="G5" s="21" t="s">
+        <v>202</v>
+      </c>
+      <c r="H5" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="I5" s="21" t="s">
+        <v>176</v>
+      </c>
+      <c r="J5" s="21" t="s">
+        <v>203</v>
+      </c>
+      <c r="K5" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="L5" s="21" t="s">
+        <v>178</v>
+      </c>
+      <c r="M5" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="N5" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="O5" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="P5" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="Q5" s="21" t="s">
+        <v>178</v>
+      </c>
+      <c r="R5" s="21" t="s">
+        <v>191</v>
+      </c>
+      <c r="S5" s="21" t="s">
+        <v>203</v>
+      </c>
+      <c r="T5" s="21" t="s">
+        <v>191</v>
+      </c>
+      <c r="U5" s="21" t="s">
+        <v>204</v>
+      </c>
+      <c r="V5" s="21" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A6" s="21" t="s">
+        <v>206</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>172</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>207</v>
+      </c>
+      <c r="D6" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" s="21" t="s">
+        <v>208</v>
+      </c>
+      <c r="F6" s="21" t="s">
+        <v>209</v>
+      </c>
+      <c r="G6" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="H6" s="21" t="s">
+        <v>210</v>
+      </c>
+      <c r="I6" s="21" t="s">
+        <v>211</v>
+      </c>
+      <c r="J6" s="21" t="s">
+        <v>190</v>
+      </c>
+      <c r="K6" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="L6" s="21" t="s">
+        <v>212</v>
+      </c>
+      <c r="M6" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="N6" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="O6" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="P6" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="Q6" s="21" t="s">
+        <v>212</v>
+      </c>
+      <c r="R6" s="21" t="s">
+        <v>212</v>
+      </c>
+      <c r="S6" s="21" t="s">
+        <v>190</v>
+      </c>
+      <c r="T6" s="21" t="s">
+        <v>212</v>
+      </c>
+      <c r="U6" s="21" t="s">
+        <v>213</v>
+      </c>
+      <c r="V6" s="21" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A7" s="21" t="s">
+        <v>215</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>172</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>216</v>
+      </c>
+      <c r="D7" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="21" t="s">
+        <v>217</v>
+      </c>
+      <c r="F7" s="21" t="s">
+        <v>218</v>
+      </c>
+      <c r="G7" s="21" t="s">
+        <v>219</v>
+      </c>
+      <c r="H7" s="21" t="s">
+        <v>220</v>
+      </c>
+      <c r="I7" s="21" t="s">
+        <v>221</v>
+      </c>
+      <c r="J7" s="21" t="s">
+        <v>177</v>
+      </c>
+      <c r="K7" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="L7" s="21" t="s">
+        <v>222</v>
+      </c>
+      <c r="M7" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="N7" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="O7" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="P7" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="Q7" s="21" t="s">
+        <v>222</v>
+      </c>
+      <c r="R7" s="21" t="s">
+        <v>223</v>
+      </c>
+      <c r="S7" s="21" t="s">
+        <v>177</v>
+      </c>
+      <c r="T7" s="21" t="s">
+        <v>223</v>
+      </c>
+      <c r="U7" s="21" t="s">
+        <v>224</v>
+      </c>
+      <c r="V7" s="21" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A8" s="21" t="s">
+        <v>226</v>
+      </c>
+      <c r="B8" s="21" t="s">
+        <v>172</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>227</v>
+      </c>
+      <c r="D8" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="21" t="s">
+        <v>228</v>
+      </c>
+      <c r="F8" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="G8" s="21" t="s">
+        <v>229</v>
+      </c>
+      <c r="H8" s="21" t="s">
+        <v>220</v>
+      </c>
+      <c r="I8" s="21" t="s">
+        <v>221</v>
+      </c>
+      <c r="J8" s="21" t="s">
+        <v>177</v>
+      </c>
+      <c r="K8" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="L8" s="21" t="s">
+        <v>222</v>
+      </c>
+      <c r="M8" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="N8" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="O8" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="P8" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="Q8" s="21" t="s">
+        <v>222</v>
+      </c>
+      <c r="R8" s="21" t="s">
+        <v>223</v>
+      </c>
+      <c r="S8" s="21" t="s">
+        <v>177</v>
+      </c>
+      <c r="T8" s="21" t="s">
+        <v>223</v>
+      </c>
+      <c r="U8" s="21" t="s">
+        <v>230</v>
+      </c>
+      <c r="V8" s="21" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A9" s="21" t="s">
+        <v>231</v>
+      </c>
+      <c r="B9" s="21" t="s">
+        <v>172</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>232</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="21" t="s">
+        <v>233</v>
+      </c>
+      <c r="F9" s="21" t="s">
+        <v>234</v>
+      </c>
+      <c r="G9" s="21" t="s">
+        <v>235</v>
+      </c>
+      <c r="H9" s="21" t="s">
+        <v>236</v>
+      </c>
+      <c r="I9" s="21" t="s">
+        <v>237</v>
+      </c>
+      <c r="J9" s="21" t="s">
+        <v>203</v>
+      </c>
+      <c r="K9" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="L9" s="21" t="s">
+        <v>238</v>
+      </c>
+      <c r="M9" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="N9" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="O9" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="P9" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="Q9" s="21" t="s">
+        <v>239</v>
+      </c>
+      <c r="R9" s="21" t="s">
+        <v>240</v>
+      </c>
+      <c r="S9" s="21" t="s">
+        <v>203</v>
+      </c>
+      <c r="T9" s="21" t="s">
+        <v>240</v>
+      </c>
+      <c r="U9" s="21" t="s">
+        <v>204</v>
+      </c>
+      <c r="V9" s="21" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A10" s="21" t="s">
+        <v>242</v>
+      </c>
+      <c r="B10" s="21" t="s">
+        <v>172</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>243</v>
+      </c>
+      <c r="D10" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" s="21" t="s">
+        <v>244</v>
+      </c>
+      <c r="F10" s="21" t="s">
+        <v>245</v>
+      </c>
+      <c r="G10" s="21" t="s">
+        <v>219</v>
+      </c>
+      <c r="H10" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="I10" s="21" t="s">
+        <v>246</v>
+      </c>
+      <c r="J10" s="21" t="s">
+        <v>177</v>
+      </c>
+      <c r="K10" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="L10" s="21" t="s">
+        <v>247</v>
+      </c>
+      <c r="M10" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="N10" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="O10" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="P10" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="Q10" s="21" t="s">
+        <v>247</v>
+      </c>
+      <c r="R10" s="21" t="s">
+        <v>248</v>
+      </c>
+      <c r="S10" s="21" t="s">
+        <v>177</v>
+      </c>
+      <c r="T10" s="21" t="s">
+        <v>248</v>
+      </c>
+      <c r="U10" s="21" t="s">
+        <v>249</v>
+      </c>
+      <c r="V10" s="21" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A11" s="21" t="s">
+        <v>251</v>
+      </c>
+      <c r="B11" s="21" t="s">
+        <v>172</v>
+      </c>
+      <c r="C11" s="21" t="s">
+        <v>252</v>
+      </c>
+      <c r="D11" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="21" t="s">
+        <v>253</v>
+      </c>
+      <c r="F11" s="21" t="s">
+        <v>254</v>
+      </c>
+      <c r="G11" s="21" t="s">
+        <v>255</v>
+      </c>
+      <c r="H11" s="21" t="s">
+        <v>256</v>
+      </c>
+      <c r="I11" s="21" t="s">
+        <v>257</v>
+      </c>
+      <c r="J11" s="21" t="s">
+        <v>177</v>
+      </c>
+      <c r="K11" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="L11" s="21" t="s">
+        <v>178</v>
+      </c>
+      <c r="M11" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="N11" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="O11" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="P11" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="Q11" s="21" t="s">
+        <v>178</v>
+      </c>
+      <c r="R11" s="21" t="s">
+        <v>180</v>
+      </c>
+      <c r="S11" s="21" t="s">
+        <v>177</v>
+      </c>
+      <c r="T11" s="21" t="s">
+        <v>180</v>
+      </c>
+      <c r="U11" s="21" t="s">
+        <v>249</v>
+      </c>
+      <c r="V11" s="21" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A12" s="21" t="s">
+        <v>258</v>
+      </c>
+      <c r="B12" s="21" t="s">
+        <v>172</v>
+      </c>
+      <c r="C12" s="21" t="s">
+        <v>259</v>
+      </c>
+      <c r="D12" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" s="21" t="s">
+        <v>260</v>
+      </c>
+      <c r="F12" s="21" t="s">
+        <v>261</v>
+      </c>
+      <c r="G12" s="21" t="s">
+        <v>262</v>
+      </c>
+      <c r="H12" s="21" t="s">
+        <v>263</v>
+      </c>
+      <c r="I12" s="21" t="s">
+        <v>264</v>
+      </c>
+      <c r="J12" s="21" t="s">
+        <v>265</v>
+      </c>
+      <c r="K12" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="L12" s="21" t="s">
+        <v>266</v>
+      </c>
+      <c r="M12" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="N12" s="21" t="s">
+        <v>267</v>
+      </c>
+      <c r="O12" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="P12" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="Q12" s="21" t="s">
+        <v>268</v>
+      </c>
+      <c r="R12" s="21" t="s">
+        <v>269</v>
+      </c>
+      <c r="S12" s="21" t="s">
+        <v>265</v>
+      </c>
+      <c r="T12" s="21" t="s">
+        <v>269</v>
+      </c>
+      <c r="U12" s="21" t="s">
+        <v>266</v>
+      </c>
+      <c r="V12" s="21" t="s">
+        <v>270</v>
       </c>
     </row>
   </sheetData>
@@ -1042,7 +2129,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
@@ -5936,4 +7023,75 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.28515625" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>3013686313</v>
+      </c>
+      <c r="B2">
+        <v>904492748</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>3013684370</v>
+      </c>
+      <c r="B3">
+        <v>904492469</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3013688560</v>
+      </c>
+      <c r="B4">
+        <v>904493578</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3013686777</v>
+      </c>
+      <c r="B5">
+        <v>904493242</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>3013686776</v>
+      </c>
+      <c r="B6">
+        <v>904493314</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
8-move non test invoices so that they are not processed, set counter to 2
</commit_message>
<xml_diff>
--- a/Resources/8-data.xlsx
+++ b/Resources/8-data.xlsx
@@ -1272,10 +1272,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V12"/>
+  <dimension ref="A1:V14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1374,40 +1374,40 @@
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
-        <v>171</v>
+        <v>183</v>
       </c>
       <c r="B2" s="21" t="s">
         <v>172</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>173</v>
+        <v>184</v>
       </c>
       <c r="D2" s="21" t="s">
         <v>25</v>
       </c>
       <c r="E2" s="21" t="s">
-        <v>174</v>
+        <v>185</v>
       </c>
       <c r="F2" s="21" t="s">
-        <v>62</v>
+        <v>186</v>
       </c>
       <c r="G2" s="21" t="s">
-        <v>175</v>
+        <v>187</v>
       </c>
       <c r="H2" s="21" t="s">
-        <v>28</v>
+        <v>188</v>
       </c>
       <c r="I2" s="21" t="s">
-        <v>176</v>
+        <v>189</v>
       </c>
       <c r="J2" s="21" t="s">
-        <v>177</v>
+        <v>190</v>
       </c>
       <c r="K2" s="21" t="s">
         <v>31</v>
       </c>
       <c r="L2" s="21" t="s">
-        <v>178</v>
+        <v>191</v>
       </c>
       <c r="M2" s="21" t="s">
         <v>179</v>
@@ -1416,51 +1416,51 @@
         <v>179</v>
       </c>
       <c r="O2" s="21" t="s">
-        <v>179</v>
+        <v>192</v>
       </c>
       <c r="P2" s="21" t="s">
         <v>179</v>
       </c>
       <c r="Q2" s="21" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="R2" s="21" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="S2" s="21" t="s">
-        <v>177</v>
+        <v>190</v>
       </c>
       <c r="T2" s="21" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="U2" s="21" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="V2" s="21" t="s">
-        <v>182</v>
+        <v>193</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
-        <v>183</v>
+        <v>194</v>
       </c>
       <c r="B3" s="21" t="s">
         <v>172</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>184</v>
+        <v>195</v>
       </c>
       <c r="D3" s="21" t="s">
         <v>25</v>
       </c>
       <c r="E3" s="21" t="s">
-        <v>185</v>
+        <v>196</v>
       </c>
       <c r="F3" s="21" t="s">
-        <v>186</v>
+        <v>62</v>
       </c>
       <c r="G3" s="21" t="s">
-        <v>187</v>
+        <v>197</v>
       </c>
       <c r="H3" s="21" t="s">
         <v>188</v>
@@ -1510,40 +1510,40 @@
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
-        <v>194</v>
+        <v>215</v>
       </c>
       <c r="B4" s="21" t="s">
         <v>172</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>195</v>
+        <v>216</v>
       </c>
       <c r="D4" s="21" t="s">
         <v>25</v>
       </c>
       <c r="E4" s="21" t="s">
-        <v>196</v>
+        <v>217</v>
       </c>
       <c r="F4" s="21" t="s">
-        <v>62</v>
+        <v>218</v>
       </c>
       <c r="G4" s="21" t="s">
-        <v>197</v>
+        <v>219</v>
       </c>
       <c r="H4" s="21" t="s">
-        <v>188</v>
+        <v>220</v>
       </c>
       <c r="I4" s="21" t="s">
-        <v>189</v>
+        <v>221</v>
       </c>
       <c r="J4" s="21" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
       <c r="K4" s="21" t="s">
         <v>31</v>
       </c>
       <c r="L4" s="21" t="s">
-        <v>191</v>
+        <v>222</v>
       </c>
       <c r="M4" s="21" t="s">
         <v>179</v>
@@ -1552,66 +1552,66 @@
         <v>179</v>
       </c>
       <c r="O4" s="21" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="P4" s="21" t="s">
         <v>179</v>
       </c>
       <c r="Q4" s="21" t="s">
-        <v>179</v>
+        <v>222</v>
       </c>
       <c r="R4" s="21" t="s">
-        <v>179</v>
+        <v>223</v>
       </c>
       <c r="S4" s="21" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
       <c r="T4" s="21" t="s">
-        <v>179</v>
+        <v>223</v>
       </c>
       <c r="U4" s="21" t="s">
-        <v>179</v>
+        <v>224</v>
       </c>
       <c r="V4" s="21" t="s">
-        <v>193</v>
+        <v>225</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
-        <v>198</v>
+        <v>242</v>
       </c>
       <c r="B5" s="21" t="s">
         <v>172</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>199</v>
+        <v>243</v>
       </c>
       <c r="D5" s="21" t="s">
         <v>25</v>
       </c>
       <c r="E5" s="21" t="s">
-        <v>200</v>
+        <v>244</v>
       </c>
       <c r="F5" s="21" t="s">
-        <v>201</v>
+        <v>245</v>
       </c>
       <c r="G5" s="21" t="s">
-        <v>202</v>
+        <v>219</v>
       </c>
       <c r="H5" s="21" t="s">
-        <v>28</v>
+        <v>108</v>
       </c>
       <c r="I5" s="21" t="s">
-        <v>176</v>
+        <v>246</v>
       </c>
       <c r="J5" s="21" t="s">
-        <v>203</v>
+        <v>177</v>
       </c>
       <c r="K5" s="21" t="s">
         <v>31</v>
       </c>
       <c r="L5" s="21" t="s">
-        <v>178</v>
+        <v>247</v>
       </c>
       <c r="M5" s="21" t="s">
         <v>179</v>
@@ -1626,187 +1626,51 @@
         <v>179</v>
       </c>
       <c r="Q5" s="21" t="s">
-        <v>178</v>
+        <v>247</v>
       </c>
       <c r="R5" s="21" t="s">
-        <v>191</v>
+        <v>248</v>
       </c>
       <c r="S5" s="21" t="s">
-        <v>203</v>
+        <v>177</v>
       </c>
       <c r="T5" s="21" t="s">
-        <v>191</v>
+        <v>248</v>
       </c>
       <c r="U5" s="21" t="s">
-        <v>204</v>
+        <v>249</v>
       </c>
       <c r="V5" s="21" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A6" s="21" t="s">
-        <v>206</v>
-      </c>
-      <c r="B6" s="21" t="s">
-        <v>172</v>
-      </c>
-      <c r="C6" s="21" t="s">
-        <v>207</v>
-      </c>
-      <c r="D6" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="E6" s="21" t="s">
-        <v>208</v>
-      </c>
-      <c r="F6" s="21" t="s">
-        <v>209</v>
-      </c>
-      <c r="G6" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="H6" s="21" t="s">
-        <v>210</v>
-      </c>
-      <c r="I6" s="21" t="s">
-        <v>211</v>
-      </c>
-      <c r="J6" s="21" t="s">
-        <v>190</v>
-      </c>
-      <c r="K6" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="L6" s="21" t="s">
-        <v>212</v>
-      </c>
-      <c r="M6" s="21" t="s">
-        <v>179</v>
-      </c>
-      <c r="N6" s="21" t="s">
-        <v>179</v>
-      </c>
-      <c r="O6" s="21" t="s">
-        <v>179</v>
-      </c>
-      <c r="P6" s="21" t="s">
-        <v>179</v>
-      </c>
-      <c r="Q6" s="21" t="s">
-        <v>212</v>
-      </c>
-      <c r="R6" s="21" t="s">
-        <v>212</v>
-      </c>
-      <c r="S6" s="21" t="s">
-        <v>190</v>
-      </c>
-      <c r="T6" s="21" t="s">
-        <v>212</v>
-      </c>
-      <c r="U6" s="21" t="s">
-        <v>213</v>
-      </c>
-      <c r="V6" s="21" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A7" s="21" t="s">
-        <v>215</v>
-      </c>
-      <c r="B7" s="21" t="s">
-        <v>172</v>
-      </c>
-      <c r="C7" s="21" t="s">
-        <v>216</v>
-      </c>
-      <c r="D7" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="E7" s="21" t="s">
-        <v>217</v>
-      </c>
-      <c r="F7" s="21" t="s">
-        <v>218</v>
-      </c>
-      <c r="G7" s="21" t="s">
-        <v>219</v>
-      </c>
-      <c r="H7" s="21" t="s">
-        <v>220</v>
-      </c>
-      <c r="I7" s="21" t="s">
-        <v>221</v>
-      </c>
-      <c r="J7" s="21" t="s">
-        <v>177</v>
-      </c>
-      <c r="K7" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="L7" s="21" t="s">
-        <v>222</v>
-      </c>
-      <c r="M7" s="21" t="s">
-        <v>179</v>
-      </c>
-      <c r="N7" s="21" t="s">
-        <v>179</v>
-      </c>
-      <c r="O7" s="21" t="s">
-        <v>179</v>
-      </c>
-      <c r="P7" s="21" t="s">
-        <v>179</v>
-      </c>
-      <c r="Q7" s="21" t="s">
-        <v>222</v>
-      </c>
-      <c r="R7" s="21" t="s">
-        <v>223</v>
-      </c>
-      <c r="S7" s="21" t="s">
-        <v>177</v>
-      </c>
-      <c r="T7" s="21" t="s">
-        <v>223</v>
-      </c>
-      <c r="U7" s="21" t="s">
-        <v>224</v>
-      </c>
-      <c r="V7" s="21" t="s">
-        <v>225</v>
+        <v>250</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="21" t="s">
-        <v>226</v>
+        <v>171</v>
       </c>
       <c r="B8" s="21" t="s">
         <v>172</v>
       </c>
       <c r="C8" s="21" t="s">
-        <v>227</v>
+        <v>173</v>
       </c>
       <c r="D8" s="21" t="s">
         <v>25</v>
       </c>
       <c r="E8" s="21" t="s">
-        <v>228</v>
+        <v>174</v>
       </c>
       <c r="F8" s="21" t="s">
         <v>62</v>
       </c>
       <c r="G8" s="21" t="s">
-        <v>229</v>
+        <v>175</v>
       </c>
       <c r="H8" s="21" t="s">
-        <v>220</v>
+        <v>28</v>
       </c>
       <c r="I8" s="21" t="s">
-        <v>221</v>
+        <v>176</v>
       </c>
       <c r="J8" s="21" t="s">
         <v>177</v>
@@ -1815,7 +1679,7 @@
         <v>31</v>
       </c>
       <c r="L8" s="21" t="s">
-        <v>222</v>
+        <v>178</v>
       </c>
       <c r="M8" s="21" t="s">
         <v>179</v>
@@ -1830,51 +1694,51 @@
         <v>179</v>
       </c>
       <c r="Q8" s="21" t="s">
-        <v>222</v>
+        <v>178</v>
       </c>
       <c r="R8" s="21" t="s">
-        <v>223</v>
+        <v>180</v>
       </c>
       <c r="S8" s="21" t="s">
         <v>177</v>
       </c>
       <c r="T8" s="21" t="s">
-        <v>223</v>
+        <v>180</v>
       </c>
       <c r="U8" s="21" t="s">
-        <v>230</v>
+        <v>181</v>
       </c>
       <c r="V8" s="21" t="s">
-        <v>225</v>
+        <v>182</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="21" t="s">
-        <v>231</v>
+        <v>198</v>
       </c>
       <c r="B9" s="21" t="s">
         <v>172</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>232</v>
+        <v>199</v>
       </c>
       <c r="D9" s="21" t="s">
         <v>25</v>
       </c>
       <c r="E9" s="21" t="s">
-        <v>233</v>
+        <v>200</v>
       </c>
       <c r="F9" s="21" t="s">
-        <v>234</v>
+        <v>201</v>
       </c>
       <c r="G9" s="21" t="s">
-        <v>235</v>
+        <v>202</v>
       </c>
       <c r="H9" s="21" t="s">
-        <v>236</v>
+        <v>28</v>
       </c>
       <c r="I9" s="21" t="s">
-        <v>237</v>
+        <v>176</v>
       </c>
       <c r="J9" s="21" t="s">
         <v>203</v>
@@ -1883,7 +1747,7 @@
         <v>31</v>
       </c>
       <c r="L9" s="21" t="s">
-        <v>238</v>
+        <v>178</v>
       </c>
       <c r="M9" s="21" t="s">
         <v>179</v>
@@ -1898,60 +1762,60 @@
         <v>179</v>
       </c>
       <c r="Q9" s="21" t="s">
-        <v>239</v>
+        <v>178</v>
       </c>
       <c r="R9" s="21" t="s">
-        <v>240</v>
+        <v>191</v>
       </c>
       <c r="S9" s="21" t="s">
         <v>203</v>
       </c>
       <c r="T9" s="21" t="s">
-        <v>240</v>
+        <v>191</v>
       </c>
       <c r="U9" s="21" t="s">
         <v>204</v>
       </c>
       <c r="V9" s="21" t="s">
-        <v>241</v>
+        <v>205</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="21" t="s">
-        <v>242</v>
+        <v>206</v>
       </c>
       <c r="B10" s="21" t="s">
         <v>172</v>
       </c>
       <c r="C10" s="21" t="s">
-        <v>243</v>
+        <v>207</v>
       </c>
       <c r="D10" s="21" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="E10" s="21" t="s">
-        <v>244</v>
+        <v>208</v>
       </c>
       <c r="F10" s="21" t="s">
-        <v>245</v>
+        <v>209</v>
       </c>
       <c r="G10" s="21" t="s">
-        <v>219</v>
+        <v>45</v>
       </c>
       <c r="H10" s="21" t="s">
-        <v>108</v>
+        <v>210</v>
       </c>
       <c r="I10" s="21" t="s">
-        <v>246</v>
+        <v>211</v>
       </c>
       <c r="J10" s="21" t="s">
-        <v>177</v>
+        <v>190</v>
       </c>
       <c r="K10" s="21" t="s">
         <v>31</v>
       </c>
       <c r="L10" s="21" t="s">
-        <v>247</v>
+        <v>212</v>
       </c>
       <c r="M10" s="21" t="s">
         <v>179</v>
@@ -1966,51 +1830,51 @@
         <v>179</v>
       </c>
       <c r="Q10" s="21" t="s">
-        <v>247</v>
+        <v>212</v>
       </c>
       <c r="R10" s="21" t="s">
-        <v>248</v>
+        <v>212</v>
       </c>
       <c r="S10" s="21" t="s">
-        <v>177</v>
+        <v>190</v>
       </c>
       <c r="T10" s="21" t="s">
-        <v>248</v>
+        <v>212</v>
       </c>
       <c r="U10" s="21" t="s">
-        <v>249</v>
+        <v>213</v>
       </c>
       <c r="V10" s="21" t="s">
-        <v>250</v>
+        <v>214</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="21" t="s">
-        <v>251</v>
+        <v>226</v>
       </c>
       <c r="B11" s="21" t="s">
         <v>172</v>
       </c>
       <c r="C11" s="21" t="s">
-        <v>252</v>
+        <v>227</v>
       </c>
       <c r="D11" s="21" t="s">
         <v>25</v>
       </c>
       <c r="E11" s="21" t="s">
-        <v>253</v>
+        <v>228</v>
       </c>
       <c r="F11" s="21" t="s">
-        <v>254</v>
+        <v>62</v>
       </c>
       <c r="G11" s="21" t="s">
-        <v>255</v>
+        <v>229</v>
       </c>
       <c r="H11" s="21" t="s">
-        <v>256</v>
+        <v>220</v>
       </c>
       <c r="I11" s="21" t="s">
-        <v>257</v>
+        <v>221</v>
       </c>
       <c r="J11" s="21" t="s">
         <v>177</v>
@@ -2019,7 +1883,7 @@
         <v>31</v>
       </c>
       <c r="L11" s="21" t="s">
-        <v>178</v>
+        <v>222</v>
       </c>
       <c r="M11" s="21" t="s">
         <v>179</v>
@@ -2034,66 +1898,66 @@
         <v>179</v>
       </c>
       <c r="Q11" s="21" t="s">
-        <v>178</v>
+        <v>222</v>
       </c>
       <c r="R11" s="21" t="s">
-        <v>180</v>
+        <v>223</v>
       </c>
       <c r="S11" s="21" t="s">
         <v>177</v>
       </c>
       <c r="T11" s="21" t="s">
-        <v>180</v>
+        <v>223</v>
       </c>
       <c r="U11" s="21" t="s">
-        <v>249</v>
+        <v>230</v>
       </c>
       <c r="V11" s="21" t="s">
-        <v>182</v>
+        <v>225</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="21" t="s">
-        <v>258</v>
+        <v>231</v>
       </c>
       <c r="B12" s="21" t="s">
         <v>172</v>
       </c>
       <c r="C12" s="21" t="s">
-        <v>259</v>
+        <v>232</v>
       </c>
       <c r="D12" s="21" t="s">
         <v>25</v>
       </c>
       <c r="E12" s="21" t="s">
-        <v>260</v>
+        <v>233</v>
       </c>
       <c r="F12" s="21" t="s">
-        <v>261</v>
+        <v>234</v>
       </c>
       <c r="G12" s="21" t="s">
-        <v>262</v>
+        <v>235</v>
       </c>
       <c r="H12" s="21" t="s">
-        <v>263</v>
+        <v>236</v>
       </c>
       <c r="I12" s="21" t="s">
-        <v>264</v>
+        <v>237</v>
       </c>
       <c r="J12" s="21" t="s">
-        <v>265</v>
+        <v>203</v>
       </c>
       <c r="K12" s="21" t="s">
         <v>31</v>
       </c>
       <c r="L12" s="21" t="s">
-        <v>266</v>
+        <v>238</v>
       </c>
       <c r="M12" s="21" t="s">
         <v>179</v>
       </c>
       <c r="N12" s="21" t="s">
-        <v>267</v>
+        <v>179</v>
       </c>
       <c r="O12" s="21" t="s">
         <v>179</v>
@@ -2102,21 +1966,157 @@
         <v>179</v>
       </c>
       <c r="Q12" s="21" t="s">
+        <v>239</v>
+      </c>
+      <c r="R12" s="21" t="s">
+        <v>240</v>
+      </c>
+      <c r="S12" s="21" t="s">
+        <v>203</v>
+      </c>
+      <c r="T12" s="21" t="s">
+        <v>240</v>
+      </c>
+      <c r="U12" s="21" t="s">
+        <v>204</v>
+      </c>
+      <c r="V12" s="21" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A13" s="21" t="s">
+        <v>251</v>
+      </c>
+      <c r="B13" s="21" t="s">
+        <v>172</v>
+      </c>
+      <c r="C13" s="21" t="s">
+        <v>252</v>
+      </c>
+      <c r="D13" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" s="21" t="s">
+        <v>253</v>
+      </c>
+      <c r="F13" s="21" t="s">
+        <v>254</v>
+      </c>
+      <c r="G13" s="21" t="s">
+        <v>255</v>
+      </c>
+      <c r="H13" s="21" t="s">
+        <v>256</v>
+      </c>
+      <c r="I13" s="21" t="s">
+        <v>257</v>
+      </c>
+      <c r="J13" s="21" t="s">
+        <v>177</v>
+      </c>
+      <c r="K13" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="L13" s="21" t="s">
+        <v>178</v>
+      </c>
+      <c r="M13" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="N13" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="O13" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="P13" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="Q13" s="21" t="s">
+        <v>178</v>
+      </c>
+      <c r="R13" s="21" t="s">
+        <v>180</v>
+      </c>
+      <c r="S13" s="21" t="s">
+        <v>177</v>
+      </c>
+      <c r="T13" s="21" t="s">
+        <v>180</v>
+      </c>
+      <c r="U13" s="21" t="s">
+        <v>249</v>
+      </c>
+      <c r="V13" s="21" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A14" s="21" t="s">
+        <v>258</v>
+      </c>
+      <c r="B14" s="21" t="s">
+        <v>172</v>
+      </c>
+      <c r="C14" s="21" t="s">
+        <v>259</v>
+      </c>
+      <c r="D14" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" s="21" t="s">
+        <v>260</v>
+      </c>
+      <c r="F14" s="21" t="s">
+        <v>261</v>
+      </c>
+      <c r="G14" s="21" t="s">
+        <v>262</v>
+      </c>
+      <c r="H14" s="21" t="s">
+        <v>263</v>
+      </c>
+      <c r="I14" s="21" t="s">
+        <v>264</v>
+      </c>
+      <c r="J14" s="21" t="s">
+        <v>265</v>
+      </c>
+      <c r="K14" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="L14" s="21" t="s">
+        <v>266</v>
+      </c>
+      <c r="M14" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="N14" s="21" t="s">
+        <v>267</v>
+      </c>
+      <c r="O14" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="P14" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="Q14" s="21" t="s">
         <v>268</v>
       </c>
-      <c r="R12" s="21" t="s">
+      <c r="R14" s="21" t="s">
         <v>269</v>
       </c>
-      <c r="S12" s="21" t="s">
+      <c r="S14" s="21" t="s">
         <v>265</v>
       </c>
-      <c r="T12" s="21" t="s">
+      <c r="T14" s="21" t="s">
         <v>269</v>
       </c>
-      <c r="U12" s="21" t="s">
+      <c r="U14" s="21" t="s">
         <v>266</v>
       </c>
-      <c r="V12" s="21" t="s">
+      <c r="V14" s="21" t="s">
         <v>270</v>
       </c>
     </row>

</xml_diff>

<commit_message>
8-updated few observations in last coloumn asNotes
</commit_message>
<xml_diff>
--- a/Resources/8-data.xlsx
+++ b/Resources/8-data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="960" yWindow="660" windowWidth="20580" windowHeight="11640"/>
+    <workbookView xWindow="960" yWindow="660" windowWidth="20580" windowHeight="11640" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="910" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="914" uniqueCount="275">
   <si>
     <t>ORDER</t>
   </si>
@@ -830,13 +830,26 @@
   </si>
   <si>
     <t xml:space="preserve"> 23.52</t>
+  </si>
+  <si>
+    <t>Disc 3 value is 10.0 in invoice</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Unit price and U/M not read properly, need to increase Y cordinates</t>
+  </si>
+  <si>
+    <t>Customer PO and Item Code naming convention differs.
+Also Net price is negative, fails to compare negative price</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -857,6 +870,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -901,7 +921,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -946,7 +966,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -960,17 +980,23 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1274,849 +1300,849 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection sqref="A1:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" style="21" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" style="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11" style="21" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.140625" style="21" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" style="21" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.140625" style="21" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.140625" style="21" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.7109375" style="21" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="28.28515625" style="21" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.28515625" style="21" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="4.85546875" style="21" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.7109375" style="21" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="6" style="21" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.5703125" style="21" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11" style="21" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.85546875" style="21" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.140625" style="21" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="18.5703125" style="21" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="17" style="21" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="30.42578125" style="21" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="14.5703125" style="21" bestFit="1" customWidth="1"/>
-    <col min="23" max="16384" width="9.140625" style="21"/>
+    <col min="1" max="1" width="12.28515625" style="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" style="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" style="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.140625" style="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" style="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.140625" style="17" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" style="17" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" style="17" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.28515625" style="17" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.28515625" style="17" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.85546875" style="17" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.7109375" style="17" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="6" style="17" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.5703125" style="17" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11" style="17" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.85546875" style="17" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.140625" style="17" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18.5703125" style="17" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17" style="17" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="30.42578125" style="17" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.5703125" style="17" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="9.140625" style="17"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="G1" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="20" t="s">
+      <c r="H1" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="20" t="s">
+      <c r="I1" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="20" t="s">
+      <c r="J1" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="K1" s="20" t="s">
+      <c r="K1" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="L1" s="20" t="s">
+      <c r="L1" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="20" t="s">
+      <c r="M1" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="N1" s="20" t="s">
+      <c r="N1" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="O1" s="20" t="s">
+      <c r="O1" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="P1" s="20" t="s">
+      <c r="P1" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="Q1" s="20" t="s">
+      <c r="Q1" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="R1" s="20" t="s">
+      <c r="R1" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="S1" s="20" t="s">
+      <c r="S1" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="T1" s="20" t="s">
+      <c r="T1" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="U1" s="20" t="s">
+      <c r="U1" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="V1" s="20" t="s">
+      <c r="V1" s="16" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="17" t="s">
         <v>183</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="17" t="s">
         <v>172</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="17" t="s">
         <v>184</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="D2" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="21" t="s">
+      <c r="E2" s="17" t="s">
         <v>185</v>
       </c>
-      <c r="F2" s="21" t="s">
+      <c r="F2" s="17" t="s">
         <v>186</v>
       </c>
-      <c r="G2" s="21" t="s">
+      <c r="G2" s="17" t="s">
         <v>187</v>
       </c>
-      <c r="H2" s="21" t="s">
+      <c r="H2" s="17" t="s">
         <v>188</v>
       </c>
-      <c r="I2" s="21" t="s">
+      <c r="I2" s="17" t="s">
         <v>189</v>
       </c>
-      <c r="J2" s="21" t="s">
+      <c r="J2" s="17" t="s">
         <v>190</v>
       </c>
-      <c r="K2" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="L2" s="21" t="s">
+      <c r="K2" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="L2" s="17" t="s">
         <v>191</v>
       </c>
-      <c r="M2" s="21" t="s">
+      <c r="M2" s="17" t="s">
         <v>179</v>
       </c>
-      <c r="N2" s="21" t="s">
+      <c r="N2" s="17" t="s">
         <v>179</v>
       </c>
-      <c r="O2" s="21" t="s">
+      <c r="O2" s="17" t="s">
         <v>192</v>
       </c>
-      <c r="P2" s="21" t="s">
+      <c r="P2" s="17" t="s">
         <v>179</v>
       </c>
-      <c r="Q2" s="21" t="s">
+      <c r="Q2" s="17" t="s">
         <v>179</v>
       </c>
-      <c r="R2" s="21" t="s">
+      <c r="R2" s="17" t="s">
         <v>179</v>
       </c>
-      <c r="S2" s="21" t="s">
+      <c r="S2" s="17" t="s">
         <v>190</v>
       </c>
-      <c r="T2" s="21" t="s">
+      <c r="T2" s="17" t="s">
         <v>179</v>
       </c>
-      <c r="U2" s="21" t="s">
+      <c r="U2" s="17" t="s">
         <v>179</v>
       </c>
-      <c r="V2" s="21" t="s">
+      <c r="V2" s="17" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="17" t="s">
         <v>194</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="17" t="s">
         <v>172</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="17" t="s">
         <v>195</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="21" t="s">
+      <c r="E3" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="F3" s="21" t="s">
+      <c r="F3" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="G3" s="21" t="s">
+      <c r="G3" s="17" t="s">
         <v>197</v>
       </c>
-      <c r="H3" s="21" t="s">
+      <c r="H3" s="17" t="s">
         <v>188</v>
       </c>
-      <c r="I3" s="21" t="s">
+      <c r="I3" s="17" t="s">
         <v>189</v>
       </c>
-      <c r="J3" s="21" t="s">
+      <c r="J3" s="17" t="s">
         <v>190</v>
       </c>
-      <c r="K3" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="L3" s="21" t="s">
+      <c r="K3" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="L3" s="17" t="s">
         <v>191</v>
       </c>
-      <c r="M3" s="21" t="s">
+      <c r="M3" s="17" t="s">
         <v>179</v>
       </c>
-      <c r="N3" s="21" t="s">
+      <c r="N3" s="17" t="s">
         <v>179</v>
       </c>
-      <c r="O3" s="21" t="s">
+      <c r="O3" s="17" t="s">
         <v>192</v>
       </c>
-      <c r="P3" s="21" t="s">
+      <c r="P3" s="17" t="s">
         <v>179</v>
       </c>
-      <c r="Q3" s="21" t="s">
+      <c r="Q3" s="17" t="s">
         <v>179</v>
       </c>
-      <c r="R3" s="21" t="s">
+      <c r="R3" s="17" t="s">
         <v>179</v>
       </c>
-      <c r="S3" s="21" t="s">
+      <c r="S3" s="17" t="s">
         <v>190</v>
       </c>
-      <c r="T3" s="21" t="s">
+      <c r="T3" s="17" t="s">
         <v>179</v>
       </c>
-      <c r="U3" s="21" t="s">
+      <c r="U3" s="17" t="s">
         <v>179</v>
       </c>
-      <c r="V3" s="21" t="s">
+      <c r="V3" s="17" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="17" t="s">
         <v>215</v>
       </c>
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="17" t="s">
         <v>172</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="17" t="s">
         <v>216</v>
       </c>
-      <c r="D4" s="21" t="s">
+      <c r="D4" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="21" t="s">
+      <c r="E4" s="17" t="s">
         <v>217</v>
       </c>
-      <c r="F4" s="21" t="s">
+      <c r="F4" s="17" t="s">
         <v>218</v>
       </c>
-      <c r="G4" s="21" t="s">
+      <c r="G4" s="17" t="s">
         <v>219</v>
       </c>
-      <c r="H4" s="21" t="s">
+      <c r="H4" s="17" t="s">
         <v>220</v>
       </c>
-      <c r="I4" s="21" t="s">
+      <c r="I4" s="17" t="s">
         <v>221</v>
       </c>
-      <c r="J4" s="21" t="s">
+      <c r="J4" s="17" t="s">
         <v>177</v>
       </c>
-      <c r="K4" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="L4" s="21" t="s">
+      <c r="K4" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="L4" s="17" t="s">
         <v>222</v>
       </c>
-      <c r="M4" s="21" t="s">
+      <c r="M4" s="17" t="s">
         <v>179</v>
       </c>
-      <c r="N4" s="21" t="s">
+      <c r="N4" s="17" t="s">
         <v>179</v>
       </c>
-      <c r="O4" s="21" t="s">
+      <c r="O4" s="17" t="s">
         <v>179</v>
       </c>
-      <c r="P4" s="21" t="s">
+      <c r="P4" s="17" t="s">
         <v>179</v>
       </c>
-      <c r="Q4" s="21" t="s">
+      <c r="Q4" s="17" t="s">
         <v>222</v>
       </c>
-      <c r="R4" s="21" t="s">
+      <c r="R4" s="17" t="s">
         <v>223</v>
       </c>
-      <c r="S4" s="21" t="s">
+      <c r="S4" s="17" t="s">
         <v>177</v>
       </c>
-      <c r="T4" s="21" t="s">
+      <c r="T4" s="17" t="s">
         <v>223</v>
       </c>
-      <c r="U4" s="21" t="s">
+      <c r="U4" s="17" t="s">
         <v>224</v>
       </c>
-      <c r="V4" s="21" t="s">
+      <c r="V4" s="17" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="17" t="s">
         <v>242</v>
       </c>
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="17" t="s">
         <v>172</v>
       </c>
-      <c r="C5" s="21" t="s">
+      <c r="C5" s="17" t="s">
         <v>243</v>
       </c>
-      <c r="D5" s="21" t="s">
+      <c r="D5" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="21" t="s">
+      <c r="E5" s="17" t="s">
         <v>244</v>
       </c>
-      <c r="F5" s="21" t="s">
+      <c r="F5" s="17" t="s">
         <v>245</v>
       </c>
-      <c r="G5" s="21" t="s">
+      <c r="G5" s="17" t="s">
         <v>219</v>
       </c>
-      <c r="H5" s="21" t="s">
+      <c r="H5" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="I5" s="21" t="s">
+      <c r="I5" s="17" t="s">
         <v>246</v>
       </c>
-      <c r="J5" s="21" t="s">
+      <c r="J5" s="17" t="s">
         <v>177</v>
       </c>
-      <c r="K5" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="L5" s="21" t="s">
+      <c r="K5" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="L5" s="17" t="s">
         <v>247</v>
       </c>
-      <c r="M5" s="21" t="s">
+      <c r="M5" s="17" t="s">
         <v>179</v>
       </c>
-      <c r="N5" s="21" t="s">
+      <c r="N5" s="17" t="s">
         <v>179</v>
       </c>
-      <c r="O5" s="21" t="s">
+      <c r="O5" s="17" t="s">
         <v>179</v>
       </c>
-      <c r="P5" s="21" t="s">
+      <c r="P5" s="17" t="s">
         <v>179</v>
       </c>
-      <c r="Q5" s="21" t="s">
+      <c r="Q5" s="17" t="s">
         <v>247</v>
       </c>
-      <c r="R5" s="21" t="s">
+      <c r="R5" s="17" t="s">
         <v>248</v>
       </c>
-      <c r="S5" s="21" t="s">
+      <c r="S5" s="17" t="s">
         <v>177</v>
       </c>
-      <c r="T5" s="21" t="s">
+      <c r="T5" s="17" t="s">
         <v>248</v>
       </c>
-      <c r="U5" s="21" t="s">
+      <c r="U5" s="17" t="s">
         <v>249</v>
       </c>
-      <c r="V5" s="21" t="s">
+      <c r="V5" s="17" t="s">
         <v>250</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A8" s="21" t="s">
+      <c r="A8" s="17" t="s">
         <v>171</v>
       </c>
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="17" t="s">
         <v>172</v>
       </c>
-      <c r="C8" s="21" t="s">
+      <c r="C8" s="17" t="s">
         <v>173</v>
       </c>
-      <c r="D8" s="21" t="s">
+      <c r="D8" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="E8" s="21" t="s">
+      <c r="E8" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="F8" s="21" t="s">
+      <c r="F8" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="G8" s="21" t="s">
+      <c r="G8" s="17" t="s">
         <v>175</v>
       </c>
-      <c r="H8" s="21" t="s">
+      <c r="H8" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="I8" s="21" t="s">
+      <c r="I8" s="17" t="s">
         <v>176</v>
       </c>
-      <c r="J8" s="21" t="s">
+      <c r="J8" s="17" t="s">
         <v>177</v>
       </c>
-      <c r="K8" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="L8" s="21" t="s">
+      <c r="K8" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="L8" s="17" t="s">
         <v>178</v>
       </c>
-      <c r="M8" s="21" t="s">
+      <c r="M8" s="17" t="s">
         <v>179</v>
       </c>
-      <c r="N8" s="21" t="s">
+      <c r="N8" s="17" t="s">
         <v>179</v>
       </c>
-      <c r="O8" s="21" t="s">
+      <c r="O8" s="17" t="s">
         <v>179</v>
       </c>
-      <c r="P8" s="21" t="s">
+      <c r="P8" s="17" t="s">
         <v>179</v>
       </c>
-      <c r="Q8" s="21" t="s">
+      <c r="Q8" s="17" t="s">
         <v>178</v>
       </c>
-      <c r="R8" s="21" t="s">
+      <c r="R8" s="17" t="s">
         <v>180</v>
       </c>
-      <c r="S8" s="21" t="s">
+      <c r="S8" s="17" t="s">
         <v>177</v>
       </c>
-      <c r="T8" s="21" t="s">
+      <c r="T8" s="17" t="s">
         <v>180</v>
       </c>
-      <c r="U8" s="21" t="s">
+      <c r="U8" s="17" t="s">
         <v>181</v>
       </c>
-      <c r="V8" s="21" t="s">
+      <c r="V8" s="17" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A9" s="21" t="s">
+      <c r="A9" s="17" t="s">
         <v>198</v>
       </c>
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="17" t="s">
         <v>172</v>
       </c>
-      <c r="C9" s="21" t="s">
+      <c r="C9" s="17" t="s">
         <v>199</v>
       </c>
-      <c r="D9" s="21" t="s">
+      <c r="D9" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="21" t="s">
+      <c r="E9" s="17" t="s">
         <v>200</v>
       </c>
-      <c r="F9" s="21" t="s">
+      <c r="F9" s="17" t="s">
         <v>201</v>
       </c>
-      <c r="G9" s="21" t="s">
+      <c r="G9" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="H9" s="21" t="s">
+      <c r="H9" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="I9" s="21" t="s">
+      <c r="I9" s="17" t="s">
         <v>176</v>
       </c>
-      <c r="J9" s="21" t="s">
+      <c r="J9" s="17" t="s">
         <v>203</v>
       </c>
-      <c r="K9" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="L9" s="21" t="s">
+      <c r="K9" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="L9" s="17" t="s">
         <v>178</v>
       </c>
-      <c r="M9" s="21" t="s">
+      <c r="M9" s="17" t="s">
         <v>179</v>
       </c>
-      <c r="N9" s="21" t="s">
+      <c r="N9" s="17" t="s">
         <v>179</v>
       </c>
-      <c r="O9" s="21" t="s">
+      <c r="O9" s="17" t="s">
         <v>179</v>
       </c>
-      <c r="P9" s="21" t="s">
+      <c r="P9" s="17" t="s">
         <v>179</v>
       </c>
-      <c r="Q9" s="21" t="s">
+      <c r="Q9" s="17" t="s">
         <v>178</v>
       </c>
-      <c r="R9" s="21" t="s">
+      <c r="R9" s="17" t="s">
         <v>191</v>
       </c>
-      <c r="S9" s="21" t="s">
+      <c r="S9" s="17" t="s">
         <v>203</v>
       </c>
-      <c r="T9" s="21" t="s">
+      <c r="T9" s="17" t="s">
         <v>191</v>
       </c>
-      <c r="U9" s="21" t="s">
+      <c r="U9" s="17" t="s">
         <v>204</v>
       </c>
-      <c r="V9" s="21" t="s">
+      <c r="V9" s="17" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A10" s="21" t="s">
+      <c r="A10" s="17" t="s">
         <v>206</v>
       </c>
-      <c r="B10" s="21" t="s">
+      <c r="B10" s="17" t="s">
         <v>172</v>
       </c>
-      <c r="C10" s="21" t="s">
+      <c r="C10" s="17" t="s">
         <v>207</v>
       </c>
-      <c r="D10" s="21" t="s">
+      <c r="D10" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="E10" s="21" t="s">
+      <c r="E10" s="17" t="s">
         <v>208</v>
       </c>
-      <c r="F10" s="21" t="s">
+      <c r="F10" s="17" t="s">
         <v>209</v>
       </c>
-      <c r="G10" s="21" t="s">
+      <c r="G10" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="H10" s="21" t="s">
+      <c r="H10" s="17" t="s">
         <v>210</v>
       </c>
-      <c r="I10" s="21" t="s">
+      <c r="I10" s="17" t="s">
         <v>211</v>
       </c>
-      <c r="J10" s="21" t="s">
+      <c r="J10" s="17" t="s">
         <v>190</v>
       </c>
-      <c r="K10" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="L10" s="21" t="s">
+      <c r="K10" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="L10" s="17" t="s">
         <v>212</v>
       </c>
-      <c r="M10" s="21" t="s">
+      <c r="M10" s="17" t="s">
         <v>179</v>
       </c>
-      <c r="N10" s="21" t="s">
+      <c r="N10" s="17" t="s">
         <v>179</v>
       </c>
-      <c r="O10" s="21" t="s">
+      <c r="O10" s="17" t="s">
         <v>179</v>
       </c>
-      <c r="P10" s="21" t="s">
+      <c r="P10" s="17" t="s">
         <v>179</v>
       </c>
-      <c r="Q10" s="21" t="s">
+      <c r="Q10" s="17" t="s">
         <v>212</v>
       </c>
-      <c r="R10" s="21" t="s">
+      <c r="R10" s="17" t="s">
         <v>212</v>
       </c>
-      <c r="S10" s="21" t="s">
+      <c r="S10" s="17" t="s">
         <v>190</v>
       </c>
-      <c r="T10" s="21" t="s">
+      <c r="T10" s="17" t="s">
         <v>212</v>
       </c>
-      <c r="U10" s="21" t="s">
+      <c r="U10" s="17" t="s">
         <v>213</v>
       </c>
-      <c r="V10" s="21" t="s">
+      <c r="V10" s="17" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A11" s="21" t="s">
+      <c r="A11" s="17" t="s">
         <v>226</v>
       </c>
-      <c r="B11" s="21" t="s">
+      <c r="B11" s="17" t="s">
         <v>172</v>
       </c>
-      <c r="C11" s="21" t="s">
+      <c r="C11" s="17" t="s">
         <v>227</v>
       </c>
-      <c r="D11" s="21" t="s">
+      <c r="D11" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="E11" s="21" t="s">
+      <c r="E11" s="17" t="s">
         <v>228</v>
       </c>
-      <c r="F11" s="21" t="s">
+      <c r="F11" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="G11" s="21" t="s">
+      <c r="G11" s="17" t="s">
         <v>229</v>
       </c>
-      <c r="H11" s="21" t="s">
+      <c r="H11" s="17" t="s">
         <v>220</v>
       </c>
-      <c r="I11" s="21" t="s">
+      <c r="I11" s="17" t="s">
         <v>221</v>
       </c>
-      <c r="J11" s="21" t="s">
+      <c r="J11" s="17" t="s">
         <v>177</v>
       </c>
-      <c r="K11" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="L11" s="21" t="s">
+      <c r="K11" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="L11" s="17" t="s">
         <v>222</v>
       </c>
-      <c r="M11" s="21" t="s">
+      <c r="M11" s="17" t="s">
         <v>179</v>
       </c>
-      <c r="N11" s="21" t="s">
+      <c r="N11" s="17" t="s">
         <v>179</v>
       </c>
-      <c r="O11" s="21" t="s">
+      <c r="O11" s="17" t="s">
         <v>179</v>
       </c>
-      <c r="P11" s="21" t="s">
+      <c r="P11" s="17" t="s">
         <v>179</v>
       </c>
-      <c r="Q11" s="21" t="s">
+      <c r="Q11" s="17" t="s">
         <v>222</v>
       </c>
-      <c r="R11" s="21" t="s">
+      <c r="R11" s="17" t="s">
         <v>223</v>
       </c>
-      <c r="S11" s="21" t="s">
+      <c r="S11" s="17" t="s">
         <v>177</v>
       </c>
-      <c r="T11" s="21" t="s">
+      <c r="T11" s="17" t="s">
         <v>223</v>
       </c>
-      <c r="U11" s="21" t="s">
+      <c r="U11" s="17" t="s">
         <v>230</v>
       </c>
-      <c r="V11" s="21" t="s">
+      <c r="V11" s="17" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A12" s="21" t="s">
+      <c r="A12" s="17" t="s">
         <v>231</v>
       </c>
-      <c r="B12" s="21" t="s">
+      <c r="B12" s="17" t="s">
         <v>172</v>
       </c>
-      <c r="C12" s="21" t="s">
+      <c r="C12" s="17" t="s">
         <v>232</v>
       </c>
-      <c r="D12" s="21" t="s">
+      <c r="D12" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="E12" s="21" t="s">
+      <c r="E12" s="17" t="s">
         <v>233</v>
       </c>
-      <c r="F12" s="21" t="s">
+      <c r="F12" s="17" t="s">
         <v>234</v>
       </c>
-      <c r="G12" s="21" t="s">
+      <c r="G12" s="17" t="s">
         <v>235</v>
       </c>
-      <c r="H12" s="21" t="s">
+      <c r="H12" s="17" t="s">
         <v>236</v>
       </c>
-      <c r="I12" s="21" t="s">
+      <c r="I12" s="17" t="s">
         <v>237</v>
       </c>
-      <c r="J12" s="21" t="s">
+      <c r="J12" s="17" t="s">
         <v>203</v>
       </c>
-      <c r="K12" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="L12" s="21" t="s">
+      <c r="K12" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="L12" s="17" t="s">
         <v>238</v>
       </c>
-      <c r="M12" s="21" t="s">
+      <c r="M12" s="17" t="s">
         <v>179</v>
       </c>
-      <c r="N12" s="21" t="s">
+      <c r="N12" s="17" t="s">
         <v>179</v>
       </c>
-      <c r="O12" s="21" t="s">
+      <c r="O12" s="17" t="s">
         <v>179</v>
       </c>
-      <c r="P12" s="21" t="s">
+      <c r="P12" s="17" t="s">
         <v>179</v>
       </c>
-      <c r="Q12" s="21" t="s">
+      <c r="Q12" s="17" t="s">
         <v>239</v>
       </c>
-      <c r="R12" s="21" t="s">
+      <c r="R12" s="17" t="s">
         <v>240</v>
       </c>
-      <c r="S12" s="21" t="s">
+      <c r="S12" s="17" t="s">
         <v>203</v>
       </c>
-      <c r="T12" s="21" t="s">
+      <c r="T12" s="17" t="s">
         <v>240</v>
       </c>
-      <c r="U12" s="21" t="s">
+      <c r="U12" s="17" t="s">
         <v>204</v>
       </c>
-      <c r="V12" s="21" t="s">
+      <c r="V12" s="17" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A13" s="21" t="s">
+      <c r="A13" s="17" t="s">
         <v>251</v>
       </c>
-      <c r="B13" s="21" t="s">
+      <c r="B13" s="17" t="s">
         <v>172</v>
       </c>
-      <c r="C13" s="21" t="s">
+      <c r="C13" s="17" t="s">
         <v>252</v>
       </c>
-      <c r="D13" s="21" t="s">
+      <c r="D13" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="E13" s="21" t="s">
+      <c r="E13" s="17" t="s">
         <v>253</v>
       </c>
-      <c r="F13" s="21" t="s">
+      <c r="F13" s="17" t="s">
         <v>254</v>
       </c>
-      <c r="G13" s="21" t="s">
+      <c r="G13" s="17" t="s">
         <v>255</v>
       </c>
-      <c r="H13" s="21" t="s">
+      <c r="H13" s="17" t="s">
         <v>256</v>
       </c>
-      <c r="I13" s="21" t="s">
+      <c r="I13" s="17" t="s">
         <v>257</v>
       </c>
-      <c r="J13" s="21" t="s">
+      <c r="J13" s="17" t="s">
         <v>177</v>
       </c>
-      <c r="K13" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="L13" s="21" t="s">
+      <c r="K13" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="L13" s="17" t="s">
         <v>178</v>
       </c>
-      <c r="M13" s="21" t="s">
+      <c r="M13" s="17" t="s">
         <v>179</v>
       </c>
-      <c r="N13" s="21" t="s">
+      <c r="N13" s="17" t="s">
         <v>179</v>
       </c>
-      <c r="O13" s="21" t="s">
+      <c r="O13" s="17" t="s">
         <v>179</v>
       </c>
-      <c r="P13" s="21" t="s">
+      <c r="P13" s="17" t="s">
         <v>179</v>
       </c>
-      <c r="Q13" s="21" t="s">
+      <c r="Q13" s="17" t="s">
         <v>178</v>
       </c>
-      <c r="R13" s="21" t="s">
+      <c r="R13" s="17" t="s">
         <v>180</v>
       </c>
-      <c r="S13" s="21" t="s">
+      <c r="S13" s="17" t="s">
         <v>177</v>
       </c>
-      <c r="T13" s="21" t="s">
+      <c r="T13" s="17" t="s">
         <v>180</v>
       </c>
-      <c r="U13" s="21" t="s">
+      <c r="U13" s="17" t="s">
         <v>249</v>
       </c>
-      <c r="V13" s="21" t="s">
+      <c r="V13" s="17" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A14" s="21" t="s">
+      <c r="A14" s="17" t="s">
         <v>258</v>
       </c>
-      <c r="B14" s="21" t="s">
+      <c r="B14" s="17" t="s">
         <v>172</v>
       </c>
-      <c r="C14" s="21" t="s">
+      <c r="C14" s="17" t="s">
         <v>259</v>
       </c>
-      <c r="D14" s="21" t="s">
+      <c r="D14" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="E14" s="21" t="s">
+      <c r="E14" s="17" t="s">
         <v>260</v>
       </c>
-      <c r="F14" s="21" t="s">
+      <c r="F14" s="17" t="s">
         <v>261</v>
       </c>
-      <c r="G14" s="21" t="s">
+      <c r="G14" s="17" t="s">
         <v>262</v>
       </c>
-      <c r="H14" s="21" t="s">
+      <c r="H14" s="17" t="s">
         <v>263</v>
       </c>
-      <c r="I14" s="21" t="s">
+      <c r="I14" s="17" t="s">
         <v>264</v>
       </c>
-      <c r="J14" s="21" t="s">
+      <c r="J14" s="17" t="s">
         <v>265</v>
       </c>
-      <c r="K14" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="L14" s="21" t="s">
+      <c r="K14" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="L14" s="17" t="s">
         <v>266</v>
       </c>
-      <c r="M14" s="21" t="s">
+      <c r="M14" s="17" t="s">
         <v>179</v>
       </c>
-      <c r="N14" s="21" t="s">
+      <c r="N14" s="17" t="s">
         <v>267</v>
       </c>
-      <c r="O14" s="21" t="s">
+      <c r="O14" s="17" t="s">
         <v>179</v>
       </c>
-      <c r="P14" s="21" t="s">
+      <c r="P14" s="17" t="s">
         <v>179</v>
       </c>
-      <c r="Q14" s="21" t="s">
+      <c r="Q14" s="17" t="s">
         <v>268</v>
       </c>
-      <c r="R14" s="21" t="s">
+      <c r="R14" s="17" t="s">
         <v>269</v>
       </c>
-      <c r="S14" s="21" t="s">
+      <c r="S14" s="17" t="s">
         <v>265</v>
       </c>
-      <c r="T14" s="21" t="s">
+      <c r="T14" s="17" t="s">
         <v>269</v>
       </c>
-      <c r="U14" s="21" t="s">
+      <c r="U14" s="17" t="s">
         <v>266</v>
       </c>
-      <c r="V14" s="21" t="s">
+      <c r="V14" s="17" t="s">
         <v>270</v>
       </c>
     </row>
@@ -2129,11 +2155,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W48"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="E1" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="U37" sqref="U37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="61.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
@@ -2155,6 +2183,7 @@
     <col min="20" max="20" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="31.28515625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="62" style="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
@@ -2224,7 +2253,9 @@
       <c r="V1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="W1" s="1"/>
+      <c r="W1" s="24" t="s">
+        <v>272</v>
+      </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
@@ -3246,7 +3277,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>904845032</v>
       </c>
@@ -3314,7 +3345,7 @@
         <v>170.78</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>904845033</v>
       </c>
@@ -3382,7 +3413,7 @@
         <v>51.72</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>904845034</v>
       </c>
@@ -3450,7 +3481,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>904845035</v>
       </c>
@@ -3518,7 +3549,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>904845040</v>
       </c>
@@ -3586,7 +3617,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>904845041</v>
       </c>
@@ -3654,7 +3685,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>904845092</v>
       </c>
@@ -3722,8 +3753,8 @@
         <v>160.27000000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A24">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A24" s="18">
         <v>904845047</v>
       </c>
       <c r="B24">
@@ -3790,7 +3821,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>904845094</v>
       </c>
@@ -3858,8 +3889,8 @@
         <v>185</v>
       </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A26">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A26" s="18">
         <v>904845083</v>
       </c>
       <c r="B26">
@@ -3926,7 +3957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>904845055</v>
       </c>
@@ -3994,7 +4025,7 @@
         <v>157.79</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>904845059</v>
       </c>
@@ -4062,7 +4093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>904845084</v>
       </c>
@@ -4130,7 +4161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>904845064</v>
       </c>
@@ -4198,75 +4229,78 @@
         <v>143</v>
       </c>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A31">
+    <row r="31" spans="1:23" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="23">
         <v>904845065</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="23">
         <v>20171023</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="23">
         <v>3013993906</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="E31">
+      <c r="E31" s="23">
         <v>14441597</v>
       </c>
-      <c r="F31" t="s">
+      <c r="F31" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="G31" t="s">
+      <c r="G31" s="23" t="s">
         <v>119</v>
       </c>
-      <c r="H31" t="s">
+      <c r="H31" s="23" t="s">
         <v>120</v>
       </c>
-      <c r="I31" t="s">
+      <c r="I31" s="23" t="s">
         <v>121</v>
       </c>
-      <c r="J31" t="s">
-        <v>30</v>
-      </c>
-      <c r="K31" t="s">
-        <v>31</v>
-      </c>
-      <c r="L31">
+      <c r="J31" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="K31" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="L31" s="23">
         <v>40</v>
       </c>
-      <c r="M31">
-        <v>0</v>
-      </c>
-      <c r="N31">
-        <v>0</v>
-      </c>
-      <c r="O31">
-        <v>0</v>
-      </c>
-      <c r="P31">
-        <v>0</v>
-      </c>
-      <c r="Q31">
-        <v>30</v>
-      </c>
-      <c r="R31">
-        <v>30</v>
-      </c>
-      <c r="S31" t="s">
-        <v>30</v>
-      </c>
-      <c r="T31" t="s">
-        <v>30</v>
-      </c>
-      <c r="U31" t="s">
-        <v>30</v>
-      </c>
-      <c r="V31">
+      <c r="M31" s="23">
+        <v>0</v>
+      </c>
+      <c r="N31" s="23">
+        <v>0</v>
+      </c>
+      <c r="O31" s="23">
+        <v>0</v>
+      </c>
+      <c r="P31" s="23">
+        <v>0</v>
+      </c>
+      <c r="Q31" s="23">
+        <v>30</v>
+      </c>
+      <c r="R31" s="23">
+        <v>30</v>
+      </c>
+      <c r="S31" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="T31" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="U31" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="V31" s="23">
         <v>32</v>
       </c>
-    </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W31" s="23" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>904845100</v>
       </c>
@@ -4334,7 +4368,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>904845071</v>
       </c>
@@ -4402,7 +4436,7 @@
         <v>418.18</v>
       </c>
     </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>904845074</v>
       </c>
@@ -4470,7 +4504,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>904845076</v>
       </c>
@@ -4538,7 +4572,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>904845077</v>
       </c>
@@ -4606,7 +4640,7 @@
         <v>82.32</v>
       </c>
     </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>904845078</v>
       </c>
@@ -4674,7 +4708,7 @@
         <v>24.5</v>
       </c>
     </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>904844974</v>
       </c>
@@ -4742,7 +4776,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>904844975</v>
       </c>
@@ -4810,7 +4844,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>904844976</v>
       </c>
@@ -4878,75 +4912,78 @@
         <v>145</v>
       </c>
     </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A41">
+    <row r="41" spans="1:23" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" s="23">
         <v>300140362</v>
       </c>
-      <c r="B41">
+      <c r="B41" s="23">
         <v>20171023</v>
       </c>
-      <c r="C41">
+      <c r="C41" s="23">
         <v>3013994716</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D41" s="23" t="s">
         <v>150</v>
       </c>
-      <c r="E41">
+      <c r="E41" s="23">
         <v>14443550</v>
       </c>
-      <c r="F41" t="s">
+      <c r="F41" s="23" t="s">
         <v>151</v>
       </c>
-      <c r="G41" t="s">
+      <c r="G41" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="H41" t="s">
+      <c r="H41" s="23" t="s">
         <v>152</v>
       </c>
-      <c r="I41" t="s">
+      <c r="I41" s="23" t="s">
         <v>153</v>
       </c>
-      <c r="J41" t="s">
-        <v>30</v>
-      </c>
-      <c r="K41" t="s">
-        <v>31</v>
-      </c>
-      <c r="L41">
+      <c r="J41" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="K41" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="L41" s="23">
         <v>115</v>
       </c>
-      <c r="M41">
-        <v>0</v>
-      </c>
-      <c r="N41">
-        <v>0</v>
-      </c>
-      <c r="O41">
-        <v>0</v>
-      </c>
-      <c r="P41">
+      <c r="M41" s="23">
+        <v>0</v>
+      </c>
+      <c r="N41" s="23">
+        <v>0</v>
+      </c>
+      <c r="O41" s="23">
+        <v>0</v>
+      </c>
+      <c r="P41" s="23">
         <v>-10</v>
       </c>
-      <c r="Q41">
+      <c r="Q41" s="23">
         <v>125</v>
       </c>
-      <c r="R41">
+      <c r="R41" s="23">
         <v>-125</v>
       </c>
-      <c r="S41" t="s">
-        <v>30</v>
-      </c>
-      <c r="T41" t="s">
-        <v>30</v>
-      </c>
-      <c r="U41" t="s">
-        <v>30</v>
-      </c>
-      <c r="V41">
+      <c r="S41" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="T41" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="U41" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="V41" s="23">
         <v>-130</v>
       </c>
-    </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W41" s="25" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="42" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>904844977</v>
       </c>
@@ -5014,7 +5051,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>904844978</v>
       </c>
@@ -5082,7 +5119,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>904844979</v>
       </c>
@@ -5150,7 +5187,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>904844980</v>
       </c>
@@ -5218,7 +5255,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>904844981</v>
       </c>
@@ -5286,75 +5323,78 @@
         <v>166</v>
       </c>
     </row>
-    <row r="47" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A47">
+    <row r="47" spans="1:23" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="23">
         <v>904844982</v>
       </c>
-      <c r="B47">
+      <c r="B47" s="23">
         <v>20171023</v>
       </c>
-      <c r="C47">
+      <c r="C47" s="23">
         <v>3013994737</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D47" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="E47">
+      <c r="E47" s="23">
         <v>14443581</v>
       </c>
-      <c r="F47" t="s">
+      <c r="F47" s="23" t="s">
         <v>166</v>
       </c>
-      <c r="G47" t="s">
+      <c r="G47" s="23" t="s">
         <v>167</v>
       </c>
-      <c r="H47" t="s">
+      <c r="H47" s="23" t="s">
         <v>168</v>
       </c>
-      <c r="I47" t="s">
+      <c r="I47" s="23" t="s">
         <v>158</v>
       </c>
-      <c r="J47" t="s">
-        <v>30</v>
-      </c>
-      <c r="K47" t="s">
-        <v>31</v>
-      </c>
-      <c r="L47">
+      <c r="J47" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="K47" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="L47" s="23">
         <v>128</v>
       </c>
-      <c r="M47">
-        <v>0</v>
-      </c>
-      <c r="N47">
-        <v>0</v>
-      </c>
-      <c r="O47">
+      <c r="M47" s="23">
+        <v>0</v>
+      </c>
+      <c r="N47" s="23">
+        <v>0</v>
+      </c>
+      <c r="O47" s="23">
         <v>100</v>
       </c>
-      <c r="P47">
-        <v>0</v>
-      </c>
-      <c r="Q47">
-        <v>0</v>
-      </c>
-      <c r="R47">
-        <v>0</v>
-      </c>
-      <c r="S47" t="s">
-        <v>30</v>
-      </c>
-      <c r="T47" t="s">
-        <v>30</v>
-      </c>
-      <c r="U47" t="s">
-        <v>30</v>
-      </c>
-      <c r="V47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="P47" s="23">
+        <v>0</v>
+      </c>
+      <c r="Q47" s="23">
+        <v>0</v>
+      </c>
+      <c r="R47" s="23">
+        <v>0</v>
+      </c>
+      <c r="S47" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="T47" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="U47" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="V47" s="23">
+        <v>0</v>
+      </c>
+      <c r="W47" s="23" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="48" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>300140363</v>
       </c>
@@ -5433,7 +5473,7 @@
   <dimension ref="A1:W23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A23"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5573,7 +5613,7 @@
       <c r="Q2" s="8">
         <v>15</v>
       </c>
-      <c r="R2" s="14">
+      <c r="R2" s="11">
         <v>180</v>
       </c>
       <c r="S2" s="9">
@@ -5641,7 +5681,7 @@
       <c r="Q3" s="8">
         <v>100</v>
       </c>
-      <c r="R3" s="14">
+      <c r="R3" s="11">
         <v>4300</v>
       </c>
       <c r="S3" s="9">
@@ -5709,7 +5749,7 @@
       <c r="Q4" s="8">
         <v>100</v>
       </c>
-      <c r="R4" s="14">
+      <c r="R4" s="11">
         <v>3200</v>
       </c>
       <c r="S4" s="9">
@@ -5726,7 +5766,7 @@
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A5" s="7">
+      <c r="A5" s="19">
         <v>904844937</v>
       </c>
       <c r="B5" s="8">
@@ -5777,7 +5817,7 @@
       <c r="Q5" s="8">
         <v>0</v>
       </c>
-      <c r="R5" s="14">
+      <c r="R5" s="11">
         <v>0</v>
       </c>
       <c r="S5" s="9">
@@ -5794,7 +5834,7 @@
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A6" s="7">
+      <c r="A6" s="19">
         <v>904844937</v>
       </c>
       <c r="B6" s="8">
@@ -5845,7 +5885,7 @@
       <c r="Q6" s="8">
         <v>0</v>
       </c>
-      <c r="R6" s="14">
+      <c r="R6" s="11">
         <v>0</v>
       </c>
       <c r="S6" s="9">
@@ -5861,71 +5901,71 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:23" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="11">
+    <row r="7" spans="1:23" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="20">
         <v>904845020</v>
       </c>
-      <c r="B7" s="11">
+      <c r="B7" s="20">
         <v>20171023</v>
       </c>
-      <c r="C7" s="11">
+      <c r="C7" s="20">
         <v>3013991893</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="E7" s="11">
+      <c r="E7" s="20">
         <v>14436525</v>
       </c>
-      <c r="F7" s="11" t="s">
+      <c r="F7" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="G7" s="11" t="s">
+      <c r="G7" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="H7" s="11" t="s">
+      <c r="H7" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="I7" s="11" t="s">
+      <c r="I7" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="J7" s="12">
+      <c r="J7" s="15">
         <v>2</v>
       </c>
-      <c r="K7" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="L7" s="11">
+      <c r="K7" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="L7" s="20">
         <v>36</v>
       </c>
-      <c r="M7" s="11">
-        <v>0</v>
-      </c>
-      <c r="N7" s="11">
-        <v>0</v>
-      </c>
-      <c r="O7" s="11">
-        <v>0</v>
-      </c>
-      <c r="P7" s="11">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="11">
+      <c r="M7" s="20">
+        <v>0</v>
+      </c>
+      <c r="N7" s="20">
+        <v>0</v>
+      </c>
+      <c r="O7" s="20">
+        <v>0</v>
+      </c>
+      <c r="P7" s="20">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="20">
         <v>36</v>
       </c>
-      <c r="R7" s="15">
+      <c r="R7" s="21">
         <v>72</v>
       </c>
-      <c r="S7" s="12">
+      <c r="S7" s="15">
         <v>2</v>
       </c>
-      <c r="T7" s="12">
+      <c r="T7" s="15">
         <v>72</v>
       </c>
-      <c r="U7" s="12">
+      <c r="U7" s="15">
         <v>10</v>
       </c>
-      <c r="V7" s="11">
+      <c r="V7" s="20">
         <v>82.02</v>
       </c>
     </row>
@@ -6066,7 +6106,7 @@
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A10" s="7">
+      <c r="A10" s="19">
         <v>904845023</v>
       </c>
       <c r="B10" s="8">
@@ -6134,7 +6174,7 @@
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A11" s="7">
+      <c r="A11" s="19">
         <v>904845023</v>
       </c>
       <c r="B11" s="8">
@@ -6676,70 +6716,70 @@
       </c>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A19" s="16">
+      <c r="A19" s="12">
         <v>904845035</v>
       </c>
-      <c r="B19" s="17">
+      <c r="B19" s="13">
         <v>20171023</v>
       </c>
-      <c r="C19" s="17">
+      <c r="C19" s="13">
         <v>3013992930</v>
       </c>
-      <c r="D19" s="17" t="s">
+      <c r="D19" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="E19" s="17">
+      <c r="E19" s="13">
         <v>14440375</v>
       </c>
-      <c r="F19" s="17" t="s">
+      <c r="F19" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="G19" s="17" t="s">
+      <c r="G19" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="H19" s="17" t="s">
+      <c r="H19" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="I19" s="17" t="s">
+      <c r="I19" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="J19" s="18">
+      <c r="J19" s="14">
         <v>2</v>
       </c>
-      <c r="K19" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="L19" s="17">
+      <c r="K19" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="L19" s="13">
         <v>64</v>
       </c>
-      <c r="M19" s="17">
-        <v>0</v>
-      </c>
-      <c r="N19" s="17">
-        <v>0</v>
-      </c>
-      <c r="O19" s="17">
-        <v>0</v>
-      </c>
-      <c r="P19" s="17">
-        <v>0</v>
-      </c>
-      <c r="Q19" s="17">
+      <c r="M19" s="13">
+        <v>0</v>
+      </c>
+      <c r="N19" s="13">
+        <v>0</v>
+      </c>
+      <c r="O19" s="13">
+        <v>0</v>
+      </c>
+      <c r="P19" s="13">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="13">
         <v>64</v>
       </c>
-      <c r="R19" s="17">
+      <c r="R19" s="13">
         <v>128</v>
       </c>
-      <c r="S19" s="18">
+      <c r="S19" s="14">
         <v>2</v>
       </c>
-      <c r="T19" s="18">
+      <c r="T19" s="14">
         <v>128</v>
       </c>
-      <c r="U19" s="18">
-        <v>30</v>
-      </c>
-      <c r="V19" s="17">
+      <c r="U19" s="14">
+        <v>30</v>
+      </c>
+      <c r="V19" s="13">
         <v>158</v>
       </c>
     </row>
@@ -6867,7 +6907,7 @@
       <c r="R21" s="8">
         <v>147</v>
       </c>
-      <c r="S21" s="19">
+      <c r="S21" s="15">
         <v>6</v>
       </c>
       <c r="T21" s="9">

</xml_diff>

<commit_message>
8- Resource File Updated
</commit_message>
<xml_diff>
--- a/Resources/8-data.xlsx
+++ b/Resources/8-data.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="820" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="805" uniqueCount="275">
   <si>
     <t>ORDER</t>
   </si>
@@ -2155,10 +2155,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="J33" sqref="J33"/>
+      <selection pane="bottomLeft" activeCell="S47" sqref="S47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="61.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3438,8 +3438,8 @@
       <c r="I19" t="s">
         <v>80</v>
       </c>
-      <c r="J19" t="s">
-        <v>30</v>
+      <c r="J19">
+        <v>1</v>
       </c>
       <c r="K19" t="s">
         <v>31</v>
@@ -3465,14 +3465,14 @@
       <c r="R19">
         <v>145</v>
       </c>
-      <c r="S19" t="s">
-        <v>30</v>
-      </c>
-      <c r="T19" t="s">
-        <v>30</v>
-      </c>
-      <c r="U19" t="s">
-        <v>30</v>
+      <c r="S19">
+        <v>1</v>
+      </c>
+      <c r="T19">
+        <v>145</v>
+      </c>
+      <c r="U19">
+        <v>0</v>
       </c>
       <c r="V19">
         <v>145</v>
@@ -3778,8 +3778,8 @@
       <c r="I24" t="s">
         <v>98</v>
       </c>
-      <c r="J24" t="s">
-        <v>30</v>
+      <c r="J24">
+        <v>1</v>
       </c>
       <c r="K24" t="s">
         <v>31</v>
@@ -3805,14 +3805,14 @@
       <c r="R24">
         <v>141</v>
       </c>
-      <c r="S24" t="s">
-        <v>30</v>
-      </c>
-      <c r="T24" t="s">
-        <v>30</v>
-      </c>
-      <c r="U24" t="s">
-        <v>30</v>
+      <c r="S24">
+        <v>1</v>
+      </c>
+      <c r="T24">
+        <v>141</v>
+      </c>
+      <c r="U24">
+        <v>0</v>
       </c>
       <c r="V24">
         <v>141</v>
@@ -4597,8 +4597,8 @@
       <c r="I36" t="s">
         <v>137</v>
       </c>
-      <c r="J36" t="s">
-        <v>30</v>
+      <c r="J36">
+        <v>6</v>
       </c>
       <c r="K36" t="s">
         <v>31</v>
@@ -4624,14 +4624,14 @@
       <c r="R36">
         <v>82.32</v>
       </c>
-      <c r="S36" t="s">
-        <v>30</v>
-      </c>
-      <c r="T36" t="s">
-        <v>30</v>
-      </c>
-      <c r="U36" t="s">
-        <v>30</v>
+      <c r="S36">
+        <v>6</v>
+      </c>
+      <c r="T36">
+        <v>82.32</v>
+      </c>
+      <c r="U36">
+        <v>0</v>
       </c>
       <c r="V36">
         <v>82.32</v>
@@ -5372,14 +5372,14 @@
       <c r="R47" s="23">
         <v>0</v>
       </c>
-      <c r="S47" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="T47" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="U47" s="23" t="s">
-        <v>30</v>
+      <c r="S47" s="23">
+        <v>1</v>
+      </c>
+      <c r="T47" s="23">
+        <v>0</v>
+      </c>
+      <c r="U47" s="23">
+        <v>0</v>
       </c>
       <c r="V47" s="23">
         <v>0</v>

</xml_diff>